<commit_message>
Mise a jour du CV + tableau de compétence
</commit_message>
<xml_diff>
--- a/public/Tableau-competenceKenji.xlsx
+++ b/public/Tableau-competenceKenji.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AFIP\SIO SLAM 2024-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenji\Documents\AFIP\portfolio\mon-portfolio\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F06C8-8A9E-4796-8DB1-28339C41149F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE8DE0D-8603-4FE2-8C2F-9616392B6FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$37</definedName>
   </definedNames>
   <calcPr calcId="101716"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -140,18 +140,6 @@
     <t>X</t>
   </si>
   <si>
-    <t xml:space="preserve"> ajout d'un bouton sélectif permettant de trier le tableau de données affiché</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ajout d'un bouton dans le tableau permettant de changer l'état des données</t>
-  </si>
-  <si>
-    <t>correction dans la base de données avec la suppression d'un paramètre qui n'est plus utilisé</t>
-  </si>
-  <si>
-    <t>ajout d'un popup permettant aux utilisateurs de proposer une modification des données à un administrateur</t>
-  </si>
-  <si>
     <t>Réalisation de petites modifications sur un site de l'entreprise : correction d'un bug où le nom des données n'apparaissait pas lors du téléchargement du PDF</t>
   </si>
   <si>
@@ -159,6 +147,75 @@
   </si>
   <si>
     <t>Réalisation d'un petit travaille en groupe pour améliorer le SEO d'un site</t>
+  </si>
+  <si>
+    <t>utilisation de Github comme plateforme de gestion de versions pour recenser et identifier toutes nos ressources numériques, y compris les codes source, la documentation technique, et les fichiers de configuration.</t>
+  </si>
+  <si>
+    <t>01/24 -&gt;04/25</t>
+  </si>
+  <si>
+    <t>12/23-&gt;04/25</t>
+  </si>
+  <si>
+    <t>J'ai créé un compte LinkedIn pour développer et gérer mon identité professionnelle en ligne.</t>
+  </si>
+  <si>
+    <t>Au cours d'un TP réalisation d'un parcage GLPI</t>
+  </si>
+  <si>
+    <t>Réalisation d'un projet fictif GSB, création d'un intranet avancé, avec gestion de documents, articles, évènement, de forums, d'utilisateurs.</t>
+  </si>
+  <si>
+    <t>10/24-&gt;01/25</t>
+  </si>
+  <si>
+    <t>02/25-&gt;04/25</t>
+  </si>
+  <si>
+    <t>Réalisation d'un projet fictif GSB, création d'une aplication mobile, gestion de stocke.</t>
+  </si>
+  <si>
+    <t>Découverte de l'architecture de thingsboard et de ses technologie (angular), pour réaliser un POC pour remonter des données de nos système pesage.</t>
+  </si>
+  <si>
+    <t>07/24-&gt;08/24</t>
+  </si>
+  <si>
+    <t>Ajout d'un input sur le site base grue pour permettre la recherche par numéro de série.</t>
+  </si>
+  <si>
+    <t>Ajout d'un bouton sur le site base grue permettant de validé ou non une fiche grue.</t>
+  </si>
+  <si>
+    <t>09/24-&gt;11/24</t>
+  </si>
+  <si>
+    <t>Création d'un site inspiré d'un autre de l'entreprise, pour gérer la personnalisation de ticket de facturation pour nos sytème de pesage pelle.</t>
+  </si>
+  <si>
+    <t>11/24-&gt;01/25</t>
+  </si>
+  <si>
+    <t>01/25-&gt;03/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ajout d'un bouton sélectif sur le site access code generator permettant de trier le tableau de données affiché</t>
+  </si>
+  <si>
+    <t>Correction dans la base de données du site base grue, fusion de 2 paramètre utiliser pour la même chose, avec la suppression d'un paramètre qui ne sert plus.</t>
+  </si>
+  <si>
+    <t>Ajout d'un popup sur le site de base grue permettant aux utilisateurs de proposer une modification des données à un administrateur</t>
+  </si>
+  <si>
+    <t>Utilisation de GitLab comme plateforme de gestion de versions pour recenser et identifier toutes nos ressources numériques, y compris les codes source, la documentation technique, et les fichiers de configuration.</t>
+  </si>
+  <si>
+    <t>Sur le site base grue refonte de la gestion des options pour les gérer comme les nomenclatures.</t>
+  </si>
+  <si>
+    <t>Ajout d'une fonctionnalité d'accès a distance sur le site access code generator.</t>
   </si>
 </sst>
 </file>
@@ -168,7 +225,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -241,6 +298,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -641,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -649,13 +717,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -664,28 +732,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -694,13 +756,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -709,46 +765,76 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -760,10 +846,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,38 +861,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -900,9 +965,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -940,9 +1005,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -975,26 +1040,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1027,26 +1075,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1223,10 +1254,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1239,83 +1270,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="33"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="51" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="52"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="37"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="16" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="46" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1338,12 +1369,12 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="53" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1352,7 +1383,7 @@
       <c r="F7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="53" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -1395,16 +1426,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="42"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1442,20 +1473,20 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="55">
+      <c r="A9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="28">
         <v>45413</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="29"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="25"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1493,14 +1524,20 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
+      <c r="A10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1538,14 +1575,22 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
+      <c r="A11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="52">
+        <v>45296</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="18"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1583,14 +1628,22 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
+      <c r="A12" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1628,14 +1681,22 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20"/>
+      <c r="A13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1673,14 +1734,14 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1718,14 +1779,14 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="20"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1763,14 +1824,14 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="20"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1808,14 +1869,14 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="20"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1853,14 +1914,14 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1898,16 +1959,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1945,20 +2006,20 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="28" t="s">
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="24" t="s">
         <v>26</v>
       </c>
       <c r="I20"/>
@@ -1998,24 +2059,24 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="53">
+      <c r="A21" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="27">
         <v>45413</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="29" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="25" t="s">
         <v>31</v>
       </c>
       <c r="I21"/>
@@ -2055,24 +2116,24 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="54">
+      <c r="A22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="51">
         <v>45323</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="29" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="25" t="s">
         <v>31</v>
       </c>
       <c r="I22"/>
@@ -2112,24 +2173,24 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="54">
-        <v>45444</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="29" t="s">
+      <c r="A23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="51">
+        <v>45474</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="25" t="s">
         <v>31</v>
       </c>
       <c r="I23"/>
@@ -2169,24 +2230,24 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="54">
-        <v>45474</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="29" t="s">
+      <c r="A24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="25" t="s">
         <v>31</v>
       </c>
       <c r="I24"/>
@@ -2226,24 +2287,24 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="29" t="s">
+      <c r="A25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="27">
+        <v>45444</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="25" t="s">
         <v>31</v>
       </c>
       <c r="I25"/>
@@ -2283,14 +2344,26 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="20"/>
+      <c r="A26" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="27">
+        <v>45413</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2327,17 +2400,23 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="52">
+        <v>45306</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2375,14 +2454,22 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20"/>
+      <c r="A28" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2419,15 +2506,17 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20"/>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="45"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2465,14 +2554,26 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20"/>
+      <c r="A30" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2510,14 +2611,24 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
+      <c r="A31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2555,14 +2666,26 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="20"/>
+      <c r="A32" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2600,14 +2723,26 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="22"/>
+      <c r="A33" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2644,15 +2779,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="24"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="18"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2689,15 +2824,15 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="18"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -2734,8 +2869,96 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+    </row>
+    <row r="37" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+      <c r="AC37"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+    </row>
     <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2780,20 +3003,22 @@
     <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
add projet mobile + update cv et tableau compétence
</commit_message>
<xml_diff>
--- a/public/Tableau-competenceKenji.xlsx
+++ b/public/Tableau-competenceKenji.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenji\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenji\Documents\AFIP\portfolio\mon-portfolio\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99605B0D-1D4D-4D42-B7BB-0E8C3481E3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937F5F6F-35A6-4979-98E2-B239C0C1CA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -662,9 +662,51 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -688,48 +730,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1112,11 +1112,11 @@
   <dimension ref="A1:AQ67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="C6" sqref="C6"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1129,56 +1129,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="28" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="29"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="43"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="11" t="s">
         <v>8</v>
       </c>
@@ -1190,22 +1190,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1228,8 +1228,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1285,16 +1285,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1552,16 +1552,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1602,7 +1602,7 @@
       <c r="A14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -1661,7 +1661,7 @@
       <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -1717,16 +1717,16 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1888,9 +1888,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="17" t="s">
-        <v>26</v>
-      </c>
+      <c r="E19" s="17"/>
       <c r="F19" s="17" t="s">
         <v>26</v>
       </c>
@@ -1949,9 +1947,7 @@
       <c r="D20" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>26</v>
-      </c>
+      <c r="E20" s="17"/>
       <c r="F20" s="17" t="s">
         <v>26</v>
       </c>
@@ -2073,6 +2069,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2080,11 +2081,6 @@
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2096,6 +2092,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3CF964BE5E9B34EB95030C40E4AA345" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="bddbe1c09382690b7287b07c00ad9565">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a9f7c678-da62-4b6b-aadc-89bc06407348" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a65d95e2258309ce9510f004f7688ef8" ns2:_="">
     <xsd:import namespace="a9f7c678-da62-4b6b-aadc-89bc06407348"/>
@@ -2239,22 +2250,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E165AEF2-9418-49EE-AA13-CC0264C91A9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19D11DBF-BFB3-4258-96AF-4D6D08B3AF8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F72C0D4-E5A9-4249-9B14-30B01B9542E2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2270,21 +2283,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19D11DBF-BFB3-4258-96AF-4D6D08B3AF8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E165AEF2-9418-49EE-AA13-CC0264C91A9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>